<commit_message>
CodingStyle and bababa revised
</commit_message>
<xml_diff>
--- a/experiment.xlsx
+++ b/experiment.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20346"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yiminchi\DOCUME~1\MobaXterm\slash\RemoteFiles\1182232_4_10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HC\DOCUME~1\MobaXterm\slash\RemoteFiles\67100_2_17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D170E3-7561-4E9B-BCF9-4103FCA65EF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16620" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="experiment" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -103,14 +102,14 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>cache line</t>
+    <t>cache line(個數)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1027,11 +1026,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1091,7 +1090,7 @@
       </c>
       <c r="L2" s="1">
         <f>(J14+J9-K9-K14)/(J2+J9+J14)</f>
-        <v>3.7159698019680429E-2</v>
+        <v>1.5360729634657647E-3</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1119,7 +1118,7 @@
       </c>
       <c r="L3" s="1">
         <f>(J10+J15-K10-K15)/(J3+J10+J15)</f>
-        <v>0.16084005634524268</v>
+        <v>2.441629787883412E-3</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1143,11 +1142,11 @@
         <v>180273</v>
       </c>
       <c r="K4">
-        <v>180273</v>
+        <v>18273</v>
       </c>
       <c r="L4" s="1">
         <f>(J11+J16-K11-K16)/(J4+J11+J16)</f>
-        <v>0.29977251538318106</v>
+        <v>5.453596497768499E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1175,7 +1174,7 @@
       </c>
       <c r="L5" s="1">
         <f>(J12+J17-K12-K17)/(J5+J12+J17)</f>
-        <v>0.2854433953219157</v>
+        <v>5.0887803326591366E-3</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1211,10 +1210,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="2">
-        <v>10368</v>
+        <v>2048</v>
       </c>
       <c r="K9" s="2">
-        <v>2048</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1233,10 +1232,10 @@
         <v>3</v>
       </c>
       <c r="J10" s="2">
-        <v>9600</v>
+        <v>1536</v>
       </c>
       <c r="K10" s="2">
-        <v>1536</v>
+        <v>768</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1255,10 +1254,10 @@
         <v>4</v>
       </c>
       <c r="J11" s="2">
-        <v>19200</v>
+        <v>3072</v>
       </c>
       <c r="K11" s="2">
-        <v>3072</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1266,10 +1265,10 @@
         <v>5</v>
       </c>
       <c r="J12" s="2">
-        <v>12800</v>
+        <v>2048</v>
       </c>
       <c r="K12" s="2">
-        <v>2048</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1288,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>82944</v>
+        <v>65536</v>
       </c>
       <c r="K14">
         <v>65536</v>
@@ -1299,7 +1298,7 @@
         <v>3</v>
       </c>
       <c r="J15">
-        <v>101376</v>
+        <v>49152</v>
       </c>
       <c r="K15">
         <v>49152</v>
@@ -1310,7 +1309,7 @@
         <v>4</v>
       </c>
       <c r="J16">
-        <v>202752</v>
+        <v>98304</v>
       </c>
       <c r="K16">
         <v>98304</v>
@@ -1321,7 +1320,7 @@
         <v>5</v>
       </c>
       <c r="J17">
-        <v>135168</v>
+        <v>65536</v>
       </c>
       <c r="K17">
         <v>65536</v>
@@ -1337,6 +1336,10 @@
       <c r="J20">
         <v>31526.03082</v>
       </c>
+      <c r="K20">
+        <f>CEILING(J20,1)</f>
+        <v>31527</v>
+      </c>
     </row>
     <row r="21" spans="7:11" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
@@ -1345,6 +1348,10 @@
       <c r="J21">
         <v>15955.5638</v>
       </c>
+      <c r="K21">
+        <f t="shared" ref="K21:K23" si="1">CEILING(J21,1)</f>
+        <v>15956</v>
+      </c>
     </row>
     <row r="22" spans="7:11" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
@@ -1353,6 +1360,10 @@
       <c r="J22">
         <v>31197.968939999999</v>
       </c>
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>31198</v>
+      </c>
     </row>
     <row r="23" spans="7:11" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
@@ -1360,6 +1371,10 @@
       </c>
       <c r="J23">
         <v>20825.910380000001</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>20826</v>
       </c>
     </row>
   </sheetData>

</xml_diff>